<commit_message>
Inclusão da tabela ajustada e cálculo do Alpha
</commit_message>
<xml_diff>
--- a/arquivos/imi-perguntas.xlsx
+++ b/arquivos/imi-perguntas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="149">
   <si>
     <t>Id</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>20 - I felt very tense while doing this activity.</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Fiquei bem à vontade enquanto fazia esta atividade.</t>
@@ -575,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -615,6 +618,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -972,201 +978,201 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="19" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="19" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="19" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="28" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="28" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="28" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="29" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="20" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="20" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="29" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="29" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="29" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="30" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6"/>
       <c r="B2" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
+        <v>124</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="D3" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="26">
+      <c r="F3" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="27">
         <v>3</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="25" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" s="24" t="s">
+      <c r="F4" s="26"/>
+      <c r="G4" s="27">
+        <v>2</v>
+      </c>
+      <c r="H4" s="28"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="26">
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27">
+        <v>1</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27">
         <v>2</v>
       </c>
-      <c r="H4" s="27"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="23" t="s">
+      <c r="H6" s="28"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26">
-        <v>1</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" s="24" t="s">
+      <c r="E7" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27">
+        <v>2</v>
+      </c>
+      <c r="H7" s="28"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27">
+        <v>2</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26">
-        <v>2</v>
-      </c>
-      <c r="H6" s="27"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26">
-        <v>2</v>
-      </c>
-      <c r="H7" s="27"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26">
-        <v>2</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" s="26">
+      <c r="E9" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="27">
         <v>3</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1184,17 +1190,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="3.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="3.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="3.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="80.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="80.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="18" width="80.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="73.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="16" width="7.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="3.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="3.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="3.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="80.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="18" width="80.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="19" width="80.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="73.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="7.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -1630,23 +1636,23 @@
       <c r="B17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>18</v>
+      <c r="C17" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G17" s="13">
         <v>14</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I17" s="12">
         <f>CONCATENATE(B17,"-","Q",A17)</f>
@@ -1663,13 +1669,13 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="13"/>
       <c r="H18" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I18" s="12">
         <f>CONCATENATE(B18,"-","Q",A18)</f>
@@ -1686,19 +1692,19 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G19" s="13">
         <v>4</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I19" s="12">
         <f>CONCATENATE(B19,"-","Q",A19)</f>
@@ -1711,17 +1717,17 @@
         <v>24</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="13"/>
       <c r="H20" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I20" s="12">
         <f>CONCATENATE(B20,"-","Q",A20)</f>
@@ -1734,19 +1740,19 @@
         <v>25</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="13"/>
       <c r="H21" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I21" s="12">
         <f>CONCATENATE(B21,"-","Q",A21)</f>
@@ -1759,19 +1765,19 @@
         <v>26</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="13"/>
       <c r="H22" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I22" s="12">
         <f>CONCATENATE(B22,"-","Q",A22)</f>
@@ -1784,19 +1790,19 @@
         <v>27</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="13"/>
       <c r="H23" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I23" s="12">
         <f>CONCATENATE(B23,"-","Q",A23)</f>
@@ -1809,19 +1815,19 @@
         <v>28</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="13"/>
       <c r="H24" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I24" s="12">
         <f>CONCATENATE(B24,"-","Q",A24)</f>
@@ -1834,23 +1840,23 @@
         <v>29</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G25" s="13">
         <v>15</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I25" s="12">
         <f>CONCATENATE(B25,"-","Q",A25)</f>
@@ -1863,25 +1869,25 @@
         <v>30</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G26" s="13">
         <v>8</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I26" s="12">
         <f>CONCATENATE(B26,"-","Q",A26)</f>
@@ -1894,23 +1900,23 @@
         <v>32</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G27" s="13">
         <v>2</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I27" s="12">
         <f>CONCATENATE(B27,"-","Q",A27)</f>
@@ -1923,17 +1929,17 @@
         <v>33</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="13"/>
       <c r="H28" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I28" s="12">
         <f>CONCATENATE(B28,"-","Q",A28)</f>
@@ -1946,23 +1952,23 @@
         <v>35</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G29" s="13">
         <v>7</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I29" s="12">
         <f>CONCATENATE(B29,"-","Q",A29)</f>
@@ -1975,17 +1981,17 @@
         <v>37</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="13"/>
       <c r="H30" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I30" s="12">
         <f>CONCATENATE(B30,"-","Q",A30)</f>
@@ -2004,13 +2010,13 @@
         <v>18</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="13"/>
       <c r="H31" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I31" s="12">
         <f>CONCATENATE(B31,"-","Q",A31)</f>
@@ -2029,13 +2035,13 @@
         <v>18</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="13"/>
       <c r="H32" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I32" s="12">
         <f>CONCATENATE(B32,"-","Q",A32)</f>
@@ -2052,19 +2058,19 @@
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F33" s="14" t="s">
         <v>106</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>107</v>
       </c>
       <c r="G33" s="13">
         <v>3</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I33" s="12">
         <f>CONCATENATE(B33,"-","Q",A33)</f>
@@ -2081,19 +2087,19 @@
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G34" s="11">
         <v>10</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I34" s="12">
         <f>CONCATENATE(B34,"-","Q",A34)</f>
@@ -2112,13 +2118,13 @@
         <v>18</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="13"/>
       <c r="H35" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I35" s="12">
         <f>CONCATENATE(B35,"-","Q",A35)</f>
@@ -2137,19 +2143,19 @@
         <v>18</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G36" s="13">
         <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I36" s="12">
         <f>CONCATENATE(B36,"-","Q",A36)</f>
@@ -2166,13 +2172,13 @@
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="13"/>
       <c r="H37" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I37" s="12">
         <f>CONCATENATE(B37,"-","Q",A37)</f>
@@ -2189,13 +2195,13 @@
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="13"/>
       <c r="H38" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I38" s="12">
         <f>CONCATENATE(B38,"-","Q",A38)</f>

</xml_diff>

<commit_message>
Análise das perguntas correlacionadas
</commit_message>
<xml_diff>
--- a/arquivos/imi-perguntas.xlsx
+++ b/arquivos/imi-perguntas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="148">
   <si>
     <t>Id</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>20 - I felt very tense while doing this activity.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Fiquei bem à vontade enquanto fazia esta atividade.</t>
@@ -578,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -618,9 +615,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -978,201 +972,201 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="20" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="20" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="29" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="29" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="29" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="30" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="19" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="19" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="19" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="28" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="28" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="28" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="29" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6"/>
       <c r="B2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="D3" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="E3" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="26">
+        <v>3</v>
+      </c>
+      <c r="H3" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="G3" s="27">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="26">
+        <v>2</v>
+      </c>
+      <c r="H4" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="26">
+        <v>1</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26">
+        <v>2</v>
+      </c>
+      <c r="H6" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26">
+        <v>2</v>
+      </c>
+      <c r="H7" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26">
+        <v>2</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="26">
         <v>3</v>
       </c>
-      <c r="H3" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27">
-        <v>2</v>
-      </c>
-      <c r="H4" s="28"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27">
-        <v>1</v>
-      </c>
-      <c r="H5" s="28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27">
-        <v>2</v>
-      </c>
-      <c r="H6" s="28"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27">
-        <v>2</v>
-      </c>
-      <c r="H7" s="28"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27">
-        <v>2</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="G9" s="27">
-        <v>3</v>
-      </c>
-      <c r="H9" s="28"/>
+      <c r="H9" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1190,17 +1184,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="16" width="3.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="17" width="3.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="3.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="80.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="18" width="80.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="19" width="80.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="16" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="73.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="17" width="7.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="15" width="3.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="3.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="3.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="80.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="80.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="18" width="80.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="15" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="73.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="16" width="7.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="19" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -1636,23 +1630,23 @@
       <c r="B17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="G17" s="13">
         <v>14</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17" s="12">
         <f>CONCATENATE(B17,"-","Q",A17)</f>
@@ -1669,13 +1663,13 @@
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="13"/>
       <c r="H18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I18" s="12">
         <f>CONCATENATE(B18,"-","Q",A18)</f>
@@ -1692,19 +1686,19 @@
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="G19" s="13">
         <v>4</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19" s="12">
         <f>CONCATENATE(B19,"-","Q",A19)</f>
@@ -1717,17 +1711,17 @@
         <v>24</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="13"/>
       <c r="H20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I20" s="12">
         <f>CONCATENATE(B20,"-","Q",A20)</f>
@@ -1740,19 +1734,19 @@
         <v>25</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="13"/>
       <c r="H21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I21" s="12">
         <f>CONCATENATE(B21,"-","Q",A21)</f>
@@ -1765,19 +1759,19 @@
         <v>26</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="13"/>
       <c r="H22" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I22" s="12">
         <f>CONCATENATE(B22,"-","Q",A22)</f>
@@ -1790,19 +1784,19 @@
         <v>27</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="13"/>
       <c r="H23" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I23" s="12">
         <f>CONCATENATE(B23,"-","Q",A23)</f>
@@ -1815,19 +1809,19 @@
         <v>28</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="13"/>
       <c r="H24" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I24" s="12">
         <f>CONCATENATE(B24,"-","Q",A24)</f>
@@ -1840,23 +1834,23 @@
         <v>29</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="F25" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="G25" s="13">
         <v>15</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I25" s="12">
         <f>CONCATENATE(B25,"-","Q",A25)</f>
@@ -1869,25 +1863,25 @@
         <v>30</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="F26" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="G26" s="13">
         <v>8</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I26" s="12">
         <f>CONCATENATE(B26,"-","Q",A26)</f>
@@ -1900,23 +1894,23 @@
         <v>32</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="F27" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="G27" s="13">
         <v>2</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I27" s="12">
         <f>CONCATENATE(B27,"-","Q",A27)</f>
@@ -1929,17 +1923,17 @@
         <v>33</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="13"/>
       <c r="H28" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I28" s="12">
         <f>CONCATENATE(B28,"-","Q",A28)</f>
@@ -1952,23 +1946,23 @@
         <v>35</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="F29" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="G29" s="13">
         <v>7</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I29" s="12">
         <f>CONCATENATE(B29,"-","Q",A29)</f>
@@ -1981,17 +1975,17 @@
         <v>37</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="13"/>
       <c r="H30" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I30" s="12">
         <f>CONCATENATE(B30,"-","Q",A30)</f>
@@ -2010,13 +2004,13 @@
         <v>18</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="13"/>
       <c r="H31" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I31" s="12">
         <f>CONCATENATE(B31,"-","Q",A31)</f>
@@ -2035,13 +2029,13 @@
         <v>18</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="13"/>
       <c r="H32" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I32" s="12">
         <f>CONCATENATE(B32,"-","Q",A32)</f>
@@ -2058,19 +2052,19 @@
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="F33" s="14" t="s">
         <v>106</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>107</v>
       </c>
       <c r="G33" s="13">
         <v>3</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I33" s="12">
         <f>CONCATENATE(B33,"-","Q",A33)</f>
@@ -2087,19 +2081,19 @@
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="F34" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="G34" s="11">
         <v>10</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I34" s="12">
         <f>CONCATENATE(B34,"-","Q",A34)</f>
@@ -2118,13 +2112,13 @@
         <v>18</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="13"/>
       <c r="H35" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I35" s="12">
         <f>CONCATENATE(B35,"-","Q",A35)</f>
@@ -2143,19 +2137,19 @@
         <v>18</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="G36" s="13">
         <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I36" s="12">
         <f>CONCATENATE(B36,"-","Q",A36)</f>
@@ -2172,13 +2166,13 @@
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="13"/>
       <c r="H37" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I37" s="12">
         <f>CONCATENATE(B37,"-","Q",A37)</f>
@@ -2195,13 +2189,13 @@
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="13"/>
       <c r="H38" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I38" s="12">
         <f>CONCATENATE(B38,"-","Q",A38)</f>

</xml_diff>